<commit_message>
Adonnai's Hours Log 3/9/15
</commit_message>
<xml_diff>
--- a/Adonnai Girma Internship Log.xlsx
+++ b/Adonnai Girma Internship Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Time In</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Optimized some files from the previous day's directory by keeping the data robust and up-to-date.</t>
+  </si>
+  <si>
+    <t>Updated the website for a countdown timer. Basically changed the background color, foreground color, and other mechanics of the website using CSS.</t>
   </si>
 </sst>
 </file>
@@ -449,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.60277777777777775</v>
       </c>
@@ -640,6 +643,9 @@
       <c r="D10" s="2">
         <f>B10-A10</f>
         <v>0.10555555555555562</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adonnai's Hours Log 3/20/15
</commit_message>
<xml_diff>
--- a/Adonnai Girma Internship Log.xlsx
+++ b/Adonnai Girma Internship Log.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adonnai\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Time In</t>
   </si>
@@ -61,6 +66,12 @@
   </si>
   <si>
     <t>Updated the website for a countdown timer. Basically changed the background color, foreground color, and other mechanics of the website using CSS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified the resizing function mechanics located in the html file. This gave the website more versatility between different screen-sizes. Hypothetically, phones, monitors, and tablets should be able to view the website with ease. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created a function that highlights text in red when a mouse hovers over it. </t>
   </si>
 </sst>
 </file>
@@ -159,6 +170,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -206,7 +220,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,7 +255,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,17 +466,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0.60416666666666663</v>
       </c>
@@ -501,10 +515,10 @@
       </c>
       <c r="G2" s="8">
         <f>SUM(D2:D50)</f>
-        <v>0.95277777777777839</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>1.1548611111111118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>0.60416666666666663</v>
       </c>
@@ -522,7 +536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>0.60416666666666663</v>
       </c>
@@ -540,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>0.6069444444444444</v>
       </c>
@@ -558,7 +572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>0.60416666666666663</v>
       </c>
@@ -576,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>0.60277777777777775</v>
       </c>
@@ -594,7 +608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>0.60277777777777775</v>
       </c>
@@ -612,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>0.60277777777777775</v>
       </c>
@@ -630,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>0.60277777777777775</v>
       </c>
@@ -648,23 +662,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="C11" s="4">
+        <v>42074</v>
+      </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+        <v>0.10902777777777772</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>0.62569444444444444</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="C12" s="4">
+        <v>42079</v>
+      </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.3055555555555558E-2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="D13" s="2">
@@ -673,7 +707,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="D14" s="2">
@@ -682,7 +716,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="D15" s="2">
@@ -691,7 +725,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="D16" s="2">
@@ -700,7 +734,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="D17" s="2">
@@ -709,7 +743,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="D18" s="2">
@@ -718,7 +752,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="D19" s="2">
@@ -727,7 +761,7 @@
       </c>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="D20" s="2">
@@ -736,7 +770,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="D21" s="2">
@@ -745,7 +779,7 @@
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="D22" s="2">
@@ -754,7 +788,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="D23" s="2">
@@ -763,7 +797,7 @@
       </c>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="D24" s="2">
@@ -772,7 +806,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="D25" s="2">
@@ -781,7 +815,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="D26" s="2">
@@ -790,7 +824,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="D27" s="2">
@@ -799,7 +833,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="D28" s="2">
@@ -808,7 +842,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="D29" s="2">
@@ -817,7 +851,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="D30" s="2">
@@ -826,7 +860,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="D31" s="2">
@@ -835,7 +869,7 @@
       </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="D32" s="2">
@@ -844,7 +878,7 @@
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="D33" s="2">
@@ -853,7 +887,7 @@
       </c>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="D34" s="2">
@@ -862,7 +896,7 @@
       </c>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="D35" s="2">
@@ -871,7 +905,7 @@
       </c>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="D36" s="2">
@@ -880,7 +914,7 @@
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="D37" s="2">
@@ -889,7 +923,7 @@
       </c>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="D38" s="2">
@@ -898,7 +932,7 @@
       </c>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="D39" s="2">
@@ -907,7 +941,7 @@
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="D40" s="2">
@@ -916,7 +950,7 @@
       </c>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="D41" s="2">
@@ -925,7 +959,7 @@
       </c>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="D42" s="2">
@@ -934,7 +968,7 @@
       </c>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="D43" s="2">
@@ -943,7 +977,7 @@
       </c>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="D44" s="2">
@@ -952,7 +986,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="D45" s="2">
@@ -961,7 +995,7 @@
       </c>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="D46" s="2">
@@ -970,7 +1004,7 @@
       </c>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="D47" s="2">
@@ -979,7 +1013,7 @@
       </c>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="D48" s="2">
@@ -988,7 +1022,7 @@
       </c>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="D49" s="2">
@@ -997,7 +1031,7 @@
       </c>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="D50" s="2">
@@ -1018,7 +1052,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1030,7 +1064,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adonnai's Hours Log 3/23/15
</commit_message>
<xml_diff>
--- a/Adonnai Girma Internship Log.xlsx
+++ b/Adonnai Girma Internship Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Time In</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Updated the website for a countdown timer. Basically changed the background color, foreground color, and other mechanics of the website using CSS.</t>
+  </si>
+  <si>
+    <t>Updated the website once again to make sure that the website is splite into boxes. The layout of these boxes are set to change according to the screen size. This is similar to how a website readjusts itself.</t>
+  </si>
+  <si>
+    <t>Changed the font color of a title, subtitle, etc. on the website to red when you hover over it. We used the hover, mouseover, and mouseout functions to accomplish this task.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tried to implement a way for text to shake using Jquery ui. </t>
   </si>
 </sst>
 </file>
@@ -452,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +510,7 @@
       </c>
       <c r="G2" s="8">
         <f>SUM(D2:D50)</f>
-        <v>0.95277777777777839</v>
+        <v>1.2458333333333342</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -648,30 +657,59 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C11" s="4">
+        <v>42074</v>
+      </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+        <v>0.10555555555555562</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C12" s="4">
+        <v>42079</v>
+      </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C13" s="4">
+        <v>42086</v>
+      </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="6"/>
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>

</xml_diff>